<commit_message>
Add status to metadata and analyses
</commit_message>
<xml_diff>
--- a/Tables/Alpha_group_significance_Family_Tribe.xlsx
+++ b/Tables/Alpha_group_significance_Family_Tribe.xlsx
@@ -418,13 +418,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>8.614959839357425</v>
+        <v>8.680848393574308</v>
       </c>
       <c r="D2" t="n">
-        <v>0.003334131483615235</v>
+        <v>0.003215712573055775</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.01667065741807617</v>
+        <v>0.01607856286527887</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -444,13 +444,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9.034050179211462</v>
+        <v>8.781362007168454</v>
       </c>
       <c r="D3" t="n">
-        <v>0.002649967047266858</v>
+        <v>0.003043238861600076</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.01667065741807617</v>
+        <v>0.01607856286527887</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1.258272058823508</v>
+        <v>1.191176470588232</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2619784198566842</v>
+        <v>0.2750923766358885</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>0.3563117592532612</v>
@@ -632,7 +632,7 @@
         <v>0.6547208460185774</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>0.6650055421020291</v>
+        <v>0.7274676066873081</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -652,13 +652,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1875</v>
+        <v>0.02083333333334281</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6650055421020291</v>
+        <v>0.8852339144731757</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0.6650055421020291</v>
+        <v>0.8852339144731757</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -678,13 +678,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>8.322238869863014</v>
+        <v>8.425941780821915</v>
       </c>
       <c r="D12" t="n">
-        <v>0.003916262078971304</v>
+        <v>0.003699050019305536</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.03592641863732656</v>
+        <v>0.03939428548774692</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -704,13 +704,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7.956994514106611</v>
+        <v>7.790360501567419</v>
       </c>
       <c r="D13" t="n">
-        <v>0.004790189151643543</v>
+        <v>0.005252571398366256</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>0.03592641863732656</v>
+        <v>0.03939428548774692</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -730,13 +730,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4.764705882352928</v>
+        <v>4.897977941176464</v>
       </c>
       <c r="D14" t="n">
-        <v>0.02904902216194074</v>
+        <v>0.02688816202716629</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>0.1452451108097037</v>
+        <v>0.1344408101358315</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -788,7 +788,7 @@
         <v>0.06757726305587061</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>0.1689431576396765</v>
+        <v>0.1784239642790366</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -808,13 +808,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3.52190476190475</v>
+        <v>3.201904761904757</v>
       </c>
       <c r="D17" t="n">
-        <v>0.06056280797430391</v>
+        <v>0.07355255978200786</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0.1689431576396765</v>
+        <v>0.1784239642790366</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -851,22 +851,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Cyprinidae (n=64)</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>Nemacheilidae (n=21)</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Tilapiinae (n=22)</t>
-        </is>
-      </c>
       <c r="C19" t="n">
-        <v>1.985832349468694</v>
+        <v>1.948608803986701</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1587773268754739</v>
+        <v>0.1627368442509667</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>0.2977074878915137</v>
+        <v>0.3051315829705624</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -877,22 +877,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Cyprinidae (n=64)</t>
+          <t>Nemacheilidae (n=21)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Nemacheilidae (n=21)</t>
+          <t>Tilapiinae (n=22)</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1.570701827242544</v>
+        <v>1.721369539551347</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2101051206577433</v>
+        <v>0.1895168505762421</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>0.3501752010962388</v>
+        <v>0.3158614176270702</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -903,7 +903,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Mugilidae (n=3)</t>
+          <t>Poeciliidae (n=2)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -912,13 +912,13 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1.181818181818187</v>
+        <v>1.320000000000007</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2769861605075796</v>
+        <v>0.2505920506856796</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>0.4040043702058401</v>
+        <v>0.3758880760285194</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -929,7 +929,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Poeciliidae (n=2)</t>
+          <t>Mugilidae (n=3)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -938,13 +938,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1.090909090909093</v>
+        <v>1.006993006993</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2962698714842828</v>
+        <v>0.3156243007353199</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>0.4040043702058401</v>
+        <v>0.4303967737299818</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -970,7 +970,7 @@
         <v>0.4142161782425236</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>0.5177702228031544</v>
+        <v>0.4779417441259887</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -981,22 +981,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Haplochrominae (n=8)</t>
+          <t>Nemacheilidae (n=21)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Tilapiinae (n=22)</t>
+          <t>Poeciliidae (n=2)</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.3717008797653989</v>
+        <v>0.7619047619047592</v>
       </c>
       <c r="D24" t="n">
-        <v>0.542078599605877</v>
+        <v>0.3827330888852269</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>0.6254753072375504</v>
+        <v>0.4779417441259887</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1007,22 +1007,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Nemacheilidae (n=21)</t>
+          <t>Haplochrominae (n=8)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Poeciliidae (n=2)</t>
+          <t>Tilapiinae (n=22)</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.2976190476190511</v>
+        <v>0.3717008797653989</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5853789284609594</v>
+        <v>0.542078599605877</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>0.6271917090653136</v>
+        <v>0.5807984995777253</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1042,13 +1042,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.01259328358207768</v>
+        <v>0.05037313432833912</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9106491299540441</v>
+        <v>0.822415259699475</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>0.9106491299540441</v>
+        <v>0.822415259699475</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>

</xml_diff>